<commit_message>
added an append data and find row function for the test automation
</commit_message>
<xml_diff>
--- a/automate_tests/moisture_data.xlsx
+++ b/automate_tests/moisture_data.xlsx
@@ -1,60 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10115"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vishwanathan/Documents/UM-1/rover/automate_tests/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A9428FF-3C0C-0A43-B6E1-43EB1B60E7EC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16040" xr2:uid="{059278BF-F95D-2644-84B8-9CE27EBFB169}"/>
+    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="16040" windowWidth="27640" xWindow="780" yWindow="960"/>
   </bookViews>
   <sheets>
-    <sheet name="avg" sheetId="1" r:id="rId1"/>
-    <sheet name="raw" sheetId="2" r:id="rId2"/>
+    <sheet name="avg" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="raw" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>Moisture Content(%)</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -70,27 +44,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+  <cellXfs count="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -390,187 +352,214 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7CBC130-6A61-B14A-AED0-D6E8C445D1DB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1">
+    <row r="1">
+      <c r="A1" t="n">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="B1" t="n">
         <v>1</v>
       </c>
-      <c r="C1">
+      <c r="C1" t="n">
         <v>2</v>
       </c>
-      <c r="D1">
+      <c r="D1" t="n">
         <v>3</v>
       </c>
-      <c r="E1">
+      <c r="E1" t="n">
         <v>4</v>
       </c>
-      <c r="F1">
+      <c r="F1" t="n">
         <v>5</v>
       </c>
-      <c r="G1">
+      <c r="G1" t="n">
         <v>6</v>
       </c>
-      <c r="H1">
+      <c r="H1" t="n">
         <v>7</v>
       </c>
-      <c r="I1">
+      <c r="I1" t="n">
         <v>8</v>
       </c>
-      <c r="J1">
+      <c r="J1" t="n">
         <v>9</v>
       </c>
-      <c r="K1">
+      <c r="K1" t="n">
         <v>10</v>
       </c>
-      <c r="L1">
+      <c r="L1" t="n">
         <v>11</v>
       </c>
-      <c r="M1">
+      <c r="M1" t="n">
         <v>12</v>
       </c>
-      <c r="N1">
+      <c r="N1" t="n">
         <v>13</v>
       </c>
-      <c r="O1">
+      <c r="O1" t="n">
         <v>14</v>
       </c>
-      <c r="P1">
+      <c r="P1" t="n">
         <v>15</v>
       </c>
-      <c r="Q1">
+      <c r="Q1" t="n">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="C10" t="s">
-        <v>0</v>
+    <row r="10">
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDBA1AA4-1A12-BE41-939A-27BD4AF4B657}">
-  <dimension ref="A1:AF1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AG11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:R1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:32" ht="34" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row customHeight="1" ht="34" r="1">
+      <c r="A1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B1" t="n">
         <v>1</v>
       </c>
-      <c r="B1">
-        <v>0</v>
-      </c>
-      <c r="C1">
-        <v>1</v>
-      </c>
-      <c r="D1">
+      <c r="C1" t="n">
         <v>2</v>
       </c>
-      <c r="E1">
+      <c r="D1" t="n">
         <v>3</v>
       </c>
-      <c r="F1">
+      <c r="E1" t="n">
         <v>4</v>
       </c>
-      <c r="G1">
+      <c r="F1" t="n">
         <v>5</v>
       </c>
-      <c r="H1">
+      <c r="G1" t="n">
         <v>6</v>
       </c>
-      <c r="I1">
+      <c r="H1" t="n">
         <v>7</v>
       </c>
-      <c r="J1">
+      <c r="I1" t="n">
         <v>8</v>
       </c>
-      <c r="K1">
+      <c r="J1" t="n">
         <v>9</v>
       </c>
-      <c r="L1">
+      <c r="K1" t="n">
         <v>10</v>
       </c>
-      <c r="M1">
+      <c r="L1" t="n">
         <v>11</v>
       </c>
-      <c r="N1">
+      <c r="M1" t="n">
         <v>12</v>
       </c>
-      <c r="O1">
+      <c r="N1" t="n">
         <v>13</v>
       </c>
-      <c r="P1">
+      <c r="O1" t="n">
         <v>14</v>
       </c>
-      <c r="Q1">
+      <c r="P1" t="n">
         <v>15</v>
       </c>
-      <c r="R1">
+      <c r="Q1" t="n">
         <v>16</v>
       </c>
-      <c r="S1">
+      <c r="R1" t="n">
         <v>17</v>
       </c>
-      <c r="T1">
+      <c r="S1" t="n">
         <v>18</v>
       </c>
-      <c r="U1">
+      <c r="T1" t="n">
         <v>19</v>
       </c>
-      <c r="V1">
+      <c r="U1" t="n">
         <v>20</v>
       </c>
-      <c r="W1">
+      <c r="V1" t="n">
         <v>21</v>
       </c>
-      <c r="X1">
+      <c r="W1" t="n">
         <v>22</v>
       </c>
-      <c r="Y1">
+      <c r="X1" t="n">
         <v>23</v>
       </c>
-      <c r="Z1">
+      <c r="Y1" t="n">
         <v>24</v>
       </c>
-      <c r="AA1">
+      <c r="Z1" t="n">
         <v>25</v>
       </c>
-      <c r="AB1">
+      <c r="AA1" t="n">
         <v>26</v>
       </c>
-      <c r="AC1">
+      <c r="AB1" t="n">
         <v>27</v>
       </c>
-      <c r="AD1">
+      <c r="AC1" t="n">
         <v>28</v>
       </c>
-      <c r="AE1">
+      <c r="AD1" t="n">
         <v>29</v>
       </c>
-      <c r="AF1">
+      <c r="AE1" t="n">
         <v>30</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="AC2" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3"/>
+    <row r="4"/>
+    <row r="5"/>
+    <row r="6"/>
+    <row r="7"/>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11">
+      <c r="F11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
switched frmo openpyxl to numpy
</commit_message>
<xml_diff>
--- a/automate_tests/moisture_data.xlsx
+++ b/automate_tests/moisture_data.xlsx
@@ -438,8 +438,8 @@
   </sheetPr>
   <dimension ref="A1:AG11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="W10" sqref="W10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -540,19 +540,54 @@
       </c>
     </row>
     <row r="2">
-      <c r="AC2" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3"/>
-    <row r="4"/>
-    <row r="5"/>
-    <row r="6"/>
-    <row r="7"/>
-    <row r="8"/>
-    <row r="9"/>
-    <row r="10"/>
+      <c r="A2" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>15</v>
+      </c>
+    </row>
     <row r="11">
+      <c r="A11" t="n">
+        <v>15</v>
+      </c>
       <c r="F11" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>

</xml_diff>